<commit_message>
change quickmethod del muti_socre, add more param change ugs, add store attribute ability change symbollearning, add dimension,refine
</commit_message>
<xml_diff>
--- a/featurebox/data/element_table.xlsx
+++ b/featurebox/data/element_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\machine learning\feature_toolbox1.0\featurebox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC50737-D3EF-4B22-A858-9877F0EB56ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C127D34E-F6AE-4150-9A53-49A65581A45D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4093" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="551">
   <si>
     <t>number</t>
   </si>
@@ -2537,88 +2537,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2930,8 +2849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BV110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change import and export
</commit_message>
<xml_diff>
--- a/featurebox/data/element_table.xlsx
+++ b/featurebox/data/element_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\machine learning\feature_toolbox1.0\featurebox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C127D34E-F6AE-4150-9A53-49A65581A45D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDA9440-DB6D-41A6-AA9A-32E951A90783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,9 +404,6 @@
     <t>cm3*mol-1</t>
   </si>
   <si>
-    <t>10^7g*cm-3</t>
-  </si>
-  <si>
     <t>M*N*m-2</t>
   </si>
   <si>
@@ -1143,9 +1140,6 @@
   </si>
   <si>
     <t>100Fm</t>
-  </si>
-  <si>
-    <t>density</t>
   </si>
   <si>
     <t>S1</t>
@@ -1843,13 +1837,21 @@
   <si>
     <t>source</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>density atomic</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>g/L</t>
+    <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2012,6 +2014,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -2467,7 +2482,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2491,6 +2506,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2847,10 +2868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BV110"/>
+  <dimension ref="A1:BV122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="BT10" sqref="BT10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2861,9 +2882,11 @@
     <col min="63" max="63" width="12.75" style="2" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="8.75" style="2" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="8.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="66" max="71" width="8.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="66" max="69" width="8.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="12.625" style="2" customWidth="1"/>
+    <col min="71" max="71" width="8.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="17.25" style="2" customWidth="1"/>
+    <col min="73" max="73" width="19.875" style="2" customWidth="1"/>
     <col min="74" max="74" width="8.75" style="2" bestFit="1" customWidth="1"/>
     <col min="75" max="16384" width="8.625" style="2"/>
   </cols>
@@ -3094,7 +3117,7 @@
     </row>
     <row r="2" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -3318,7 +3341,7 @@
     </row>
     <row r="3" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -3366,10 +3389,10 @@
         <v>29</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>30</v>
@@ -3542,7 +3565,7 @@
     </row>
     <row r="4" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>83</v>
@@ -3637,124 +3660,124 @@
         <v>106</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="E5" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="H5" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="K5" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="N5" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="O5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="Q5" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="R5" s="5" t="s">
+      <c r="U5" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="AD5" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="X5" s="5" t="s">
+      <c r="AE5" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="AH5" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="AI5" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="Y5" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="AA5" s="5" t="s">
+      <c r="AK5" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="AL5" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="AM5" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="AN5" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="AB5" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="AC5" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="AD5" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="AE5" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="AF5" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="AG5" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="AH5" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="AI5" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="AJ5" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="AK5" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="AL5" s="5" t="s">
+      <c r="AO5" s="5" t="s">
         <v>430</v>
-      </c>
-      <c r="AM5" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="AN5" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="AO5" s="5" t="s">
-        <v>432</v>
       </c>
       <c r="AP5" s="5" t="s">
         <v>107</v>
@@ -3769,94 +3792,94 @@
         <v>110</v>
       </c>
       <c r="AT5" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="AU5" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="AV5" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="AW5" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="AX5" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="AY5" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="AU5" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="AV5" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="AW5" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="AX5" s="5" t="s">
+      <c r="AZ5" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="AY5" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="AZ5" s="5" t="s">
-        <v>401</v>
-      </c>
       <c r="BA5" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="BB5" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="BC5" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="BD5" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="BE5" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="BF5" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="BG5" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="BH5" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="BD5" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="BE5" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="BF5" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="BG5" s="5" t="s">
+      <c r="BI5" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="BJ5" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="BK5" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="BH5" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="BI5" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="BJ5" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="BK5" s="5" t="s">
-        <v>382</v>
-      </c>
       <c r="BL5" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="BM5" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="BN5" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="BO5" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="BP5" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="BQ5" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="BR5" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="BS5" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="BT5" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="BU5" s="5" t="s">
-        <v>372</v>
+        <v>549</v>
       </c>
       <c r="BV5" s="5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
-    <row r="6" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:74" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>111</v>
       </c>
@@ -4073,240 +4096,240 @@
       <c r="BT6" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="BU6" s="5" t="s">
+      <c r="BU6" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="BV6" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="BV6" s="5" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="W7" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="X7" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="Z7" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="AA7" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="AG7" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="AK7" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="AL7" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="AM7" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>519</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>520</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>523</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>525</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>526</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="V7" s="5" t="s">
-        <v>528</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="Y7" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="Z7" s="5" t="s">
+      <c r="AN7" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="AA7" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="AB7" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="AC7" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="AD7" s="5" t="s">
-        <v>529</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="AF7" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="AG7" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="AH7" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="AI7" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="AJ7" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="AK7" s="5" t="s">
+      <c r="AO7" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="AL7" s="5" t="s">
+      <c r="AP7" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="AQ7" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="AR7" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="AS7" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="AT7" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="AM7" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="AN7" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="AO7" s="5" t="s">
+      <c r="AU7" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="AP7" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="AQ7" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="AR7" s="5" t="s">
+      <c r="AV7" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="AW7" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="AX7" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="AY7" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="AZ7" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="BA7" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="BB7" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="BC7" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="BD7" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="BE7" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="BF7" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="AS7" s="5" t="s">
+      <c r="BG7" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="BH7" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="BI7" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="BJ7" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="BK7" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="BL7" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="BM7" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="BN7" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="BO7" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="BP7" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="BQ7" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="BR7" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="BS7" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="AT7" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="AU7" s="5" t="s">
-        <v>537</v>
-      </c>
-      <c r="AV7" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="AW7" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="AX7" s="5" t="s">
-        <v>498</v>
-      </c>
-      <c r="AY7" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="AZ7" s="5" t="s">
-        <v>501</v>
-      </c>
-      <c r="BA7" s="5" t="s">
-        <v>505</v>
-      </c>
-      <c r="BB7" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="BC7" s="5" t="s">
-        <v>538</v>
-      </c>
-      <c r="BD7" s="5" t="s">
-        <v>539</v>
-      </c>
-      <c r="BE7" s="5" t="s">
-        <v>540</v>
-      </c>
-      <c r="BF7" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="BG7" s="5" t="s">
+      <c r="BT7" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="BH7" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="BI7" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="BJ7" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="BK7" s="5" t="s">
-        <v>542</v>
-      </c>
-      <c r="BL7" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="BM7" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="BN7" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="BO7" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="BP7" s="5" t="s">
-        <v>514</v>
-      </c>
-      <c r="BQ7" s="5" t="s">
+      <c r="BU7" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="BV7" s="5" t="s">
         <v>515</v>
-      </c>
-      <c r="BR7" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="BS7" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="BT7" s="5" t="s">
-        <v>543</v>
-      </c>
-      <c r="BU7" s="5" t="s">
-        <v>545</v>
-      </c>
-      <c r="BV7" s="5" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>112</v>
@@ -4318,115 +4341,115 @@
         <v>112</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>376</v>
-      </c>
       <c r="I8" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="T8" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="N8" s="5" t="s">
+      <c r="U8" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="V8" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="W8" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="AE8" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF8" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG8" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI8" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ8" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="P8" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="W8" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="Y8" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA8" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB8" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="AC8" s="5" t="s">
+      <c r="AK8" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL8" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM8" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AN8" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="AO8" s="5" t="s">
         <v>390</v>
-      </c>
-      <c r="AD8" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="AE8" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="AF8" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="AG8" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH8" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="AI8" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AJ8" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="AK8" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="AL8" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM8" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="AN8" s="5" t="s">
-        <v>544</v>
-      </c>
-      <c r="AO8" s="5" t="s">
-        <v>392</v>
       </c>
       <c r="AP8" s="5" t="s">
         <v>107</v>
@@ -4441,96 +4464,96 @@
         <v>110</v>
       </c>
       <c r="AT8" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="AU8" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="AV8" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="AV8" s="5" t="s">
-        <v>495</v>
-      </c>
       <c r="AW8" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AX8" s="5" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="AY8" s="5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AZ8" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="BA8" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="BB8" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="BD8" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE8" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="BF8" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="BG8" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="BH8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="BI8" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="BJ8" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="BK8" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="BL8" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM8" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN8" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="BB8" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="BC8" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="BD8" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="BE8" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="BF8" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="BG8" s="5" t="s">
+      <c r="BO8" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="BP8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="BQ8" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="BH8" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="BI8" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="BJ8" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="BK8" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="BL8" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="BM8" s="5" t="s">
+      <c r="BR8" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="BN8" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="BO8" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="BP8" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ8" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="BR8" s="5" t="s">
+      <c r="BS8" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="BS8" s="5" t="s">
+      <c r="BT8" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="BT8" s="5" t="s">
-        <v>164</v>
-      </c>
       <c r="BU8" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="BV8" s="5" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="9" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>112</v>
@@ -4542,70 +4565,70 @@
         <v>112</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="L9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z9" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AA9" s="5" t="s">
         <v>98</v>
@@ -4614,16 +4637,16 @@
         <v>98</v>
       </c>
       <c r="AC9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AD9" s="5" t="s">
         <v>98</v>
       </c>
       <c r="AE9" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AF9" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AG9" s="5" t="s">
         <v>98</v>
@@ -4635,13 +4658,13 @@
         <v>98</v>
       </c>
       <c r="AJ9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>98</v>
@@ -4677,7 +4700,7 @@
         <v>98</v>
       </c>
       <c r="AX9" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="AY9" s="5" t="s">
         <v>98</v>
@@ -4686,75 +4709,75 @@
         <v>98</v>
       </c>
       <c r="BA9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BB9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BC9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BD9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BE9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BF9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BG9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BH9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BI9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BJ9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BK9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BL9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BM9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BN9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BO9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="BP9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="BQ9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BR9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BS9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BT9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BU9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BV9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:74" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:74" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>112</v>
@@ -4790,7 +4813,7 @@
         <v>2</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N10" s="5">
         <v>5</v>
@@ -4799,7 +4822,7 @@
         <v>3</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q10" s="5">
         <v>5</v>
@@ -4808,7 +4831,7 @@
         <v>2</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T10" s="5">
         <v>5</v>
@@ -4820,25 +4843,25 @@
         <v>5</v>
       </c>
       <c r="W10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC10" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="X10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="Y10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="Z10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="AA10" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="AB10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="AC10" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="AD10" s="5">
         <v>5</v>
@@ -4859,7 +4882,7 @@
         <v>5</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AK10" s="5">
         <v>5</v>
@@ -4904,7 +4927,7 @@
         <v>5</v>
       </c>
       <c r="AY10" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AZ10" s="5">
         <v>2</v>
@@ -4934,7 +4957,7 @@
         <v>1</v>
       </c>
       <c r="BI10" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="BJ10" s="5">
         <v>2</v>
@@ -4952,42 +4975,42 @@
         <v>1</v>
       </c>
       <c r="BO10" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="BP10" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="BQ10" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="BR10" s="5">
         <v>5</v>
       </c>
       <c r="BS10" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="BT10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="BU10" s="5">
+        <v>172</v>
+      </c>
+      <c r="BU10" s="9">
         <v>1</v>
       </c>
       <c r="BV10" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>177</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I11" s="2">
         <v>4.7</v>
@@ -5118,19 +5141,22 @@
       <c r="BT11" s="2">
         <v>11210</v>
       </c>
+      <c r="BU11" s="8">
+        <v>8.9899999999999994E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I12" s="2">
         <v>4.242</v>
@@ -5252,19 +5278,22 @@
       <c r="BT12" s="2">
         <v>22424</v>
       </c>
+      <c r="BU12" s="8">
+        <v>0.17849999999999999</v>
+      </c>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="C13" s="6">
         <v>3</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
@@ -5458,22 +5487,22 @@
       <c r="BT13" s="2">
         <v>12.97</v>
       </c>
-      <c r="BU13" s="2">
-        <v>1.1000000000000001</v>
+      <c r="BU13" s="8">
+        <v>535</v>
       </c>
     </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="C14" s="6">
         <v>4</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E14" s="2">
         <v>3</v>
@@ -5673,25 +5702,25 @@
       <c r="BT14" s="2">
         <v>4.8766999999999996</v>
       </c>
-      <c r="BU14" s="2">
-        <v>2.5</v>
+      <c r="BU14" s="8">
+        <v>1848</v>
       </c>
       <c r="BV14" s="2">
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="C15" s="6">
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I15" s="2">
         <v>5.0599999999999996</v>
@@ -5858,22 +5887,22 @@
       <c r="BT15" s="2">
         <v>4.3943000000000003</v>
       </c>
-      <c r="BU15" s="1">
-        <v>9.9999999999999994E-12</v>
+      <c r="BU15" s="8">
+        <v>2460</v>
       </c>
     </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="C16" s="6">
         <v>6</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I16" s="2">
         <v>2.464</v>
@@ -6034,22 +6063,22 @@
       <c r="BT16" s="2">
         <v>5.3146000000000004</v>
       </c>
-      <c r="BU16" s="2">
-        <v>0.01</v>
+      <c r="BU16" s="8">
+        <v>2260</v>
       </c>
     </row>
-    <row r="17" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="C17" s="6">
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I17" s="2">
         <v>3.8610000000000002</v>
@@ -6195,19 +6224,22 @@
       <c r="BT17" s="2">
         <v>11197</v>
       </c>
+      <c r="BU17" s="8">
+        <v>1.2509999999999999</v>
+      </c>
     </row>
-    <row r="18" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="C18" s="6">
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I18" s="2">
         <v>5.4029999999999996</v>
@@ -6353,19 +6385,22 @@
       <c r="BT18" s="2">
         <v>11196</v>
       </c>
+      <c r="BU18" s="8">
+        <v>1.429</v>
+      </c>
     </row>
-    <row r="19" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="C19" s="6">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I19" s="2">
         <v>5.5</v>
@@ -6511,19 +6546,22 @@
       <c r="BT19" s="2">
         <v>11202</v>
       </c>
+      <c r="BU19" s="8">
+        <v>1.696</v>
+      </c>
     </row>
-    <row r="20" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="C20" s="6">
         <v>10</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I20" s="2">
         <v>4.4290000000000003</v>
@@ -6648,19 +6686,22 @@
       <c r="BT20" s="2">
         <v>22420</v>
       </c>
+      <c r="BU20" s="8">
+        <v>0.9</v>
+      </c>
     </row>
-    <row r="21" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="C21" s="6">
         <v>11</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E21" s="2">
         <v>2</v>
@@ -6854,25 +6895,25 @@
       <c r="BT21" s="2">
         <v>23.75</v>
       </c>
-      <c r="BU21" s="2">
-        <v>2.1</v>
+      <c r="BU21" s="8">
+        <v>968</v>
       </c>
       <c r="BV21" s="2">
         <v>0.69</v>
       </c>
     </row>
-    <row r="22" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="C22" s="6">
         <v>12</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E22" s="2">
         <v>3</v>
@@ -7069,25 +7110,25 @@
       <c r="BT22" s="2">
         <v>13.984</v>
       </c>
-      <c r="BU22" s="2">
-        <v>2.2999999999999998</v>
+      <c r="BU22" s="8">
+        <v>1738</v>
       </c>
       <c r="BV22" s="2">
         <v>260</v>
       </c>
     </row>
-    <row r="23" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="C23" s="6">
         <v>13</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
@@ -7287,25 +7328,25 @@
       <c r="BT23" s="2">
         <v>9.99</v>
       </c>
-      <c r="BU23" s="2">
-        <v>3.8</v>
+      <c r="BU23" s="8">
+        <v>2700</v>
       </c>
       <c r="BV23" s="2">
         <v>245</v>
       </c>
     </row>
-    <row r="24" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="C24" s="6">
         <v>14</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I24" s="2">
         <v>5.4309000000000003</v>
@@ -7481,22 +7522,22 @@
       <c r="BT24" s="2">
         <v>12.054</v>
       </c>
-      <c r="BU24" s="2">
-        <v>1E-4</v>
+      <c r="BU24" s="8">
+        <v>2330</v>
       </c>
     </row>
-    <row r="25" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>205</v>
       </c>
       <c r="C25" s="6">
         <v>15</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I25" s="2">
         <v>11.45</v>
@@ -7660,22 +7701,22 @@
       <c r="BT25" s="2">
         <v>16.991</v>
       </c>
-      <c r="BU25" s="2">
-        <v>1</v>
+      <c r="BU25" s="8">
+        <v>1823</v>
       </c>
     </row>
-    <row r="26" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="C26" s="6">
         <v>16</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I26" s="2">
         <v>10.436999999999999</v>
@@ -7830,22 +7871,22 @@
       <c r="BT26" s="2">
         <v>16.356999999999999</v>
       </c>
-      <c r="BU26" s="1">
-        <v>1E-22</v>
+      <c r="BU26" s="8">
+        <v>1960</v>
       </c>
     </row>
-    <row r="27" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>209</v>
       </c>
       <c r="C27" s="6">
         <v>17</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I27" s="2">
         <v>6.2234999999999996</v>
@@ -8000,22 +8041,22 @@
       <c r="BT27" s="2">
         <v>11030</v>
       </c>
-      <c r="BU27" s="2">
-        <v>1.0000000000000001E-9</v>
+      <c r="BU27" s="8">
+        <v>3.214</v>
       </c>
     </row>
-    <row r="28" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="C28" s="6">
         <v>18</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I28" s="2">
         <v>5.2560000000000002</v>
@@ -8140,13 +8181,16 @@
       <c r="BT28" s="2">
         <v>22392</v>
       </c>
+      <c r="BU28" s="8">
+        <v>1.784</v>
+      </c>
     </row>
-    <row r="29" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C29" s="6">
         <v>19</v>
@@ -8340,25 +8384,25 @@
       <c r="BT29" s="2">
         <v>45.68</v>
       </c>
-      <c r="BU29" s="2">
-        <v>1.4</v>
+      <c r="BU29" s="8">
+        <v>856</v>
       </c>
       <c r="BV29" s="2">
         <v>0.36299999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>213</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>214</v>
       </c>
       <c r="C30" s="6">
         <v>20</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E30" s="2">
         <v>1</v>
@@ -8561,25 +8605,25 @@
       <c r="BT30" s="2">
         <v>25.856999999999999</v>
       </c>
-      <c r="BU30" s="2">
-        <v>2.9</v>
+      <c r="BU30" s="8">
+        <v>1550</v>
       </c>
       <c r="BV30" s="2">
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="C31" s="6">
         <v>21</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E31" s="2">
         <v>3</v>
@@ -8779,25 +8823,25 @@
       <c r="BT31" s="2">
         <v>15.061</v>
       </c>
-      <c r="BU31" s="2">
-        <v>0.18</v>
+      <c r="BU31" s="8">
+        <v>2985</v>
       </c>
       <c r="BV31" s="2">
         <v>750</v>
       </c>
     </row>
-    <row r="32" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="C32" s="6">
         <v>22</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E32" s="2">
         <v>3</v>
@@ -9000,25 +9044,25 @@
       <c r="BT32" s="2">
         <v>10.621</v>
       </c>
-      <c r="BU32" s="2">
-        <v>0.25</v>
+      <c r="BU32" s="8">
+        <v>4507</v>
       </c>
       <c r="BV32" s="2">
         <v>716</v>
       </c>
     </row>
-    <row r="33" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="C33" s="6">
         <v>23</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -9218,25 +9262,25 @@
       <c r="BT33" s="2">
         <v>8.3374000000000006</v>
       </c>
-      <c r="BU33" s="2">
-        <v>0.5</v>
+      <c r="BU33" s="8">
+        <v>6110</v>
       </c>
       <c r="BV33" s="2">
         <v>628</v>
       </c>
     </row>
-    <row r="34" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="C34" s="6">
         <v>24</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E34" s="2">
         <v>2</v>
@@ -9439,28 +9483,28 @@
       <c r="BT34" s="2">
         <v>7.2317</v>
       </c>
-      <c r="BU34" s="2">
-        <v>0.79</v>
+      <c r="BU34" s="8">
+        <v>7140</v>
       </c>
       <c r="BV34" s="2">
         <v>1120</v>
       </c>
     </row>
-    <row r="35" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="C35" s="6">
         <v>25</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
@@ -9645,25 +9689,25 @@
       <c r="BT35" s="2">
         <v>7.3544999999999998</v>
       </c>
-      <c r="BU35" s="2">
-        <v>6.2E-2</v>
+      <c r="BU35" s="8">
+        <v>7470</v>
       </c>
       <c r="BV35" s="2">
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="C36" s="6">
         <v>26</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E36" s="2">
         <v>2</v>
@@ -9869,25 +9913,25 @@
       <c r="BT36" s="2">
         <v>7.0922999999999998</v>
       </c>
-      <c r="BU36" s="2">
-        <v>1</v>
+      <c r="BU36" s="8">
+        <v>7874</v>
       </c>
       <c r="BV36" s="2">
         <v>490</v>
       </c>
     </row>
-    <row r="37" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>228</v>
       </c>
       <c r="C37" s="6">
         <v>27</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E37" s="2">
         <v>3</v>
@@ -10090,25 +10134,25 @@
       <c r="BT37" s="2">
         <v>6.62</v>
       </c>
-      <c r="BU37" s="2">
-        <v>1.7</v>
+      <c r="BU37" s="8">
+        <v>8900</v>
       </c>
       <c r="BV37" s="2">
         <v>700</v>
       </c>
     </row>
-    <row r="38" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>229</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>230</v>
       </c>
       <c r="C38" s="6">
         <v>28</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E38" s="2">
         <v>1</v>
@@ -10308,25 +10352,25 @@
       <c r="BT38" s="2">
         <v>6.5888</v>
       </c>
-      <c r="BU38" s="2">
-        <v>1.4</v>
+      <c r="BU38" s="8">
+        <v>8908</v>
       </c>
       <c r="BV38" s="2">
         <v>700</v>
       </c>
     </row>
-    <row r="39" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="C39" s="6">
         <v>29</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E39" s="2">
         <v>1</v>
@@ -10526,25 +10570,25 @@
       <c r="BT39" s="2">
         <v>7.0922000000000001</v>
       </c>
-      <c r="BU39" s="2">
-        <v>5.9</v>
+      <c r="BU39" s="8">
+        <v>8920</v>
       </c>
       <c r="BV39" s="2">
         <v>874</v>
       </c>
     </row>
-    <row r="40" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="C40" s="6">
         <v>30</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E40" s="2">
         <v>3</v>
@@ -10741,28 +10785,28 @@
       <c r="BT40" s="2">
         <v>9.157</v>
       </c>
-      <c r="BU40" s="2">
-        <v>1.7</v>
+      <c r="BU40" s="8">
+        <v>7140</v>
       </c>
       <c r="BV40" s="2">
         <v>412</v>
       </c>
     </row>
-    <row r="41" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>236</v>
       </c>
       <c r="C41" s="6">
         <v>31</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H41" s="2">
         <v>11</v>
@@ -10941,25 +10985,25 @@
       <c r="BT41" s="2">
         <v>11.808999999999999</v>
       </c>
-      <c r="BU41" s="2">
-        <v>0.71</v>
+      <c r="BU41" s="8">
+        <v>5904</v>
       </c>
       <c r="BV41" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>237</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>238</v>
       </c>
       <c r="C42" s="6">
         <v>32</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E42" s="2">
         <v>4</v>
@@ -11138,22 +11182,22 @@
       <c r="BT42" s="2">
         <v>13.645</v>
       </c>
-      <c r="BU42" s="2">
-        <v>2.0000000000000001E-4</v>
+      <c r="BU42" s="8">
+        <v>5323</v>
       </c>
     </row>
-    <row r="43" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="C43" s="6">
         <v>33</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I43" s="2">
         <v>3.7597999999999998</v>
@@ -11323,25 +11367,25 @@
       <c r="BT43" s="2">
         <v>13.082000000000001</v>
       </c>
-      <c r="BU43" s="2">
-        <v>0.33</v>
+      <c r="BU43" s="8">
+        <v>5727</v>
       </c>
       <c r="BV43" s="2">
         <v>1440</v>
       </c>
     </row>
-    <row r="44" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="C44" s="6">
         <v>34</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I44" s="2">
         <v>9.0540000000000003</v>
@@ -11508,22 +11552,25 @@
       <c r="BT44" s="2">
         <v>16.387</v>
       </c>
+      <c r="BU44" s="8">
+        <v>4819</v>
+      </c>
       <c r="BV44" s="2">
         <v>736</v>
       </c>
     </row>
-    <row r="45" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="C45" s="6">
         <v>35</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I45" s="2">
         <v>6.7264999999999997</v>
@@ -11678,22 +11725,22 @@
       <c r="BT45" s="2">
         <v>25.61</v>
       </c>
-      <c r="BU45" s="1">
-        <v>1.0000000000000001E-17</v>
+      <c r="BU45" s="8">
+        <v>3120</v>
       </c>
     </row>
-    <row r="46" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>246</v>
       </c>
       <c r="C46" s="6">
         <v>36</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I46" s="2">
         <v>5.7060000000000004</v>
@@ -11821,19 +11868,22 @@
       <c r="BT46" s="2">
         <v>22350</v>
       </c>
+      <c r="BU46" s="8">
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="47" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="C47" s="6">
         <v>37</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E47" s="2">
         <v>2</v>
@@ -12018,25 +12068,25 @@
       <c r="BT47" s="2">
         <v>55.787999999999997</v>
       </c>
-      <c r="BU47" s="2">
-        <v>0.83</v>
+      <c r="BU47" s="8">
+        <v>1532</v>
       </c>
       <c r="BV47" s="2">
         <v>0.216</v>
       </c>
     </row>
-    <row r="48" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="C48" s="6">
         <v>38</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E48" s="2">
         <v>1</v>
@@ -12236,22 +12286,22 @@
       <c r="BT48" s="2">
         <v>33.316000000000003</v>
       </c>
-      <c r="BU48" s="2">
-        <v>0.77</v>
+      <c r="BU48" s="8">
+        <v>2630</v>
       </c>
     </row>
-    <row r="49" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C49" s="6">
         <v>39</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E49" s="2">
         <v>3</v>
@@ -12451,25 +12501,25 @@
       <c r="BT49" s="2">
         <v>19.881</v>
       </c>
-      <c r="BU49" s="2">
-        <v>0.18</v>
+      <c r="BU49" s="8">
+        <v>4472</v>
       </c>
       <c r="BV49" s="2">
         <v>589</v>
       </c>
     </row>
-    <row r="50" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>252</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>253</v>
       </c>
       <c r="C50" s="6">
         <v>40</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E50" s="2">
         <v>3</v>
@@ -12669,25 +12719,25 @@
       <c r="BT50" s="2">
         <v>14.010999999999999</v>
       </c>
-      <c r="BU50" s="2">
-        <v>0.24</v>
+      <c r="BU50" s="8">
+        <v>6511</v>
       </c>
       <c r="BV50" s="2">
         <v>650</v>
       </c>
     </row>
-    <row r="51" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="C51" s="6">
         <v>41</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E51" s="2">
         <v>2</v>
@@ -12887,25 +12937,25 @@
       <c r="BT51" s="2">
         <v>10.840999999999999</v>
       </c>
-      <c r="BU51" s="2">
-        <v>0.67</v>
+      <c r="BU51" s="8">
+        <v>8570</v>
       </c>
       <c r="BV51" s="2">
         <v>736</v>
       </c>
     </row>
-    <row r="52" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>257</v>
       </c>
       <c r="C52" s="6">
         <v>42</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E52" s="2">
         <v>2</v>
@@ -13105,25 +13155,25 @@
       <c r="BT52" s="2">
         <v>9.3339999999999996</v>
       </c>
-      <c r="BU52" s="2">
-        <v>2</v>
+      <c r="BU52" s="8">
+        <v>10280</v>
       </c>
       <c r="BV52" s="2">
         <v>1500</v>
       </c>
     </row>
-    <row r="53" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C53" s="6">
         <v>43</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E53" s="2">
         <v>3</v>
@@ -13290,22 +13340,22 @@
       <c r="BT53" s="2">
         <v>8.4347826090000009</v>
       </c>
-      <c r="BU53" s="2">
-        <v>0.5</v>
+      <c r="BU53" s="8">
+        <v>11500</v>
       </c>
     </row>
-    <row r="54" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="C54" s="6">
         <v>44</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E54" s="2">
         <v>3</v>
@@ -13505,25 +13555,25 @@
       <c r="BT54" s="2">
         <v>8.1706000000000003</v>
       </c>
-      <c r="BU54" s="2">
-        <v>1.4</v>
+      <c r="BU54" s="8">
+        <v>12370</v>
       </c>
       <c r="BV54" s="2">
         <v>2160</v>
       </c>
     </row>
-    <row r="55" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>262</v>
       </c>
       <c r="C55" s="6">
         <v>45</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E55" s="2">
         <v>1</v>
@@ -13723,25 +13773,25 @@
       <c r="BT55" s="2">
         <v>8.2654999999999994</v>
       </c>
-      <c r="BU55" s="2">
-        <v>2.2999999999999998</v>
+      <c r="BU55" s="8">
+        <v>12450</v>
       </c>
       <c r="BV55" s="2">
         <v>1100</v>
       </c>
     </row>
-    <row r="56" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>264</v>
       </c>
       <c r="C56" s="6">
         <v>46</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E56" s="2">
         <v>1</v>
@@ -13941,25 +13991,25 @@
       <c r="BT56" s="2">
         <v>8.8513999999999999</v>
       </c>
-      <c r="BU56" s="2">
-        <v>1</v>
+      <c r="BU56" s="8">
+        <v>12023</v>
       </c>
       <c r="BV56" s="2">
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>266</v>
       </c>
       <c r="C57" s="6">
         <v>47</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E57" s="2">
         <v>1</v>
@@ -14159,25 +14209,25 @@
       <c r="BT57" s="2">
         <v>10.282999999999999</v>
       </c>
-      <c r="BU57" s="2">
-        <v>6.2</v>
+      <c r="BU57" s="8">
+        <v>10490</v>
       </c>
       <c r="BV57" s="2">
         <v>24.5</v>
       </c>
     </row>
-    <row r="58" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>267</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>268</v>
       </c>
       <c r="C58" s="6">
         <v>48</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E58" s="2">
         <v>3</v>
@@ -14374,25 +14424,25 @@
       <c r="BT58" s="2">
         <v>12.996</v>
       </c>
-      <c r="BU58" s="2">
-        <v>1.4</v>
+      <c r="BU58" s="8">
+        <v>8650</v>
       </c>
       <c r="BV58" s="2">
         <v>203</v>
       </c>
     </row>
-    <row r="59" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>270</v>
       </c>
       <c r="C59" s="6">
         <v>49</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E59" s="2">
         <v>6</v>
@@ -14580,25 +14630,25 @@
       <c r="BT59" s="2">
         <v>15.707000000000001</v>
       </c>
-      <c r="BU59" s="2">
-        <v>1.2</v>
+      <c r="BU59" s="8">
+        <v>7310</v>
       </c>
       <c r="BV59" s="2">
         <v>8.83</v>
       </c>
     </row>
-    <row r="60" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="C60" s="6">
         <v>50</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E60" s="2">
         <v>4</v>
@@ -14801,25 +14851,25 @@
       <c r="BT60" s="2">
         <v>16.239000000000001</v>
       </c>
-      <c r="BU60" s="2">
-        <v>0.91</v>
+      <c r="BU60" s="8">
+        <v>7310</v>
       </c>
       <c r="BV60" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="C61" s="6">
         <v>51</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E61" s="2">
         <v>7</v>
@@ -15010,25 +15060,25 @@
       <c r="BT61" s="2">
         <v>18.181000000000001</v>
       </c>
-      <c r="BU61" s="2">
-        <v>0.25</v>
+      <c r="BU61" s="8">
+        <v>6697</v>
       </c>
       <c r="BV61" s="2">
         <v>294</v>
       </c>
     </row>
-    <row r="62" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="C62" s="6">
         <v>52</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I62" s="2">
         <v>4.4572000000000003</v>
@@ -15201,25 +15251,25 @@
       <c r="BT62" s="2">
         <v>20.449000000000002</v>
       </c>
-      <c r="BU62" s="2">
-        <v>1E-3</v>
+      <c r="BU62" s="8">
+        <v>6240</v>
       </c>
       <c r="BV62" s="2">
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>278</v>
       </c>
       <c r="C63" s="6">
         <v>53</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I63" s="2">
         <v>7.1802000000000001</v>
@@ -15374,22 +15424,22 @@
       <c r="BT63" s="2">
         <v>25.689</v>
       </c>
-      <c r="BU63" s="1">
-        <v>1E-14</v>
+      <c r="BU63" s="8">
+        <v>4940</v>
       </c>
     </row>
-    <row r="64" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>280</v>
       </c>
       <c r="C64" s="6">
         <v>54</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I64" s="2">
         <v>6.2023000000000001</v>
@@ -15514,19 +15564,22 @@
       <c r="BT64" s="2">
         <v>22300</v>
       </c>
+      <c r="BU64" s="8">
+        <v>5.9</v>
+      </c>
     </row>
-    <row r="65" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>282</v>
       </c>
       <c r="C65" s="6">
         <v>55</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E65" s="2">
         <v>2</v>
@@ -15711,25 +15764,25 @@
       <c r="BT65" s="2">
         <v>70.731999999999999</v>
       </c>
-      <c r="BU65" s="2">
-        <v>0.5</v>
+      <c r="BU65" s="8">
+        <v>1879</v>
       </c>
       <c r="BV65" s="2">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>284</v>
       </c>
       <c r="C66" s="6">
         <v>56</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E66" s="2">
         <v>2</v>
@@ -15923,25 +15976,25 @@
       <c r="BT66" s="2">
         <v>39.125</v>
       </c>
-      <c r="BU66" s="2">
-        <v>0.28999999999999998</v>
+      <c r="BU66" s="8">
+        <v>3510</v>
       </c>
     </row>
-    <row r="67" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>285</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="C67" s="6">
         <v>57</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F67" s="2">
         <v>1</v>
@@ -15950,7 +16003,7 @@
         <v>2</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I67" s="2">
         <v>3.7719999999999998</v>
@@ -16141,28 +16194,28 @@
       <c r="BT67" s="2">
         <v>22.600999999999999</v>
       </c>
-      <c r="BU67" s="2">
-        <v>0.16</v>
+      <c r="BU67" s="8">
+        <v>6146</v>
       </c>
       <c r="BV67" s="2">
         <v>363</v>
       </c>
     </row>
-    <row r="68" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="C68" s="6">
         <v>58</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F68" s="2">
         <v>2</v>
@@ -16356,34 +16409,34 @@
       <c r="BT68" s="2">
         <v>20.946999999999999</v>
       </c>
-      <c r="BU68" s="2">
-        <v>0.14000000000000001</v>
+      <c r="BU68" s="8">
+        <v>6689</v>
       </c>
       <c r="BV68" s="2">
         <v>412</v>
       </c>
     </row>
-    <row r="69" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>291</v>
       </c>
       <c r="C69" s="6">
         <v>59</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F69" s="2">
         <v>2</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I69" s="2">
         <v>3.6724999999999999</v>
@@ -16574,34 +16627,34 @@
       <c r="BT69" s="2">
         <v>21.221</v>
       </c>
-      <c r="BU69" s="2">
-        <v>0.14000000000000001</v>
+      <c r="BU69" s="8">
+        <v>6640</v>
       </c>
       <c r="BV69" s="2">
         <v>481</v>
       </c>
     </row>
-    <row r="70" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>293</v>
       </c>
       <c r="C70" s="6">
         <v>60</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F70" s="2">
         <v>2</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I70" s="2">
         <v>3.6579999999999999</v>
@@ -16792,28 +16845,28 @@
       <c r="BT70" s="2">
         <v>20.577000000000002</v>
       </c>
-      <c r="BU70" s="2">
-        <v>0.16</v>
+      <c r="BU70" s="8">
+        <v>7010</v>
       </c>
       <c r="BV70" s="2">
         <v>265</v>
       </c>
     </row>
-    <row r="71" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>294</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>295</v>
       </c>
       <c r="C71" s="6">
         <v>61</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L71" s="2">
         <v>1.85</v>
@@ -16992,28 +17045,28 @@
       <c r="BT71" s="2">
         <v>19.96145374</v>
       </c>
-      <c r="BU71" s="2">
-        <v>0.13</v>
+      <c r="BU71" s="8">
+        <v>7264</v>
       </c>
     </row>
-    <row r="72" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>297</v>
       </c>
       <c r="C72" s="6">
         <v>62</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I72" s="2">
         <v>3.621</v>
@@ -17201,25 +17254,25 @@
       <c r="BT72" s="2">
         <v>20.449000000000002</v>
       </c>
-      <c r="BU72" s="2">
-        <v>0.11</v>
+      <c r="BU72" s="8">
+        <v>7353</v>
       </c>
       <c r="BV72" s="2">
         <v>441</v>
       </c>
     </row>
-    <row r="73" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>299</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>300</v>
       </c>
       <c r="C73" s="6">
         <v>63</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E73" s="2">
         <v>2</v>
@@ -17416,22 +17469,22 @@
       <c r="BT73" s="2">
         <v>28.978999999999999</v>
       </c>
-      <c r="BU73" s="2">
-        <v>0.11</v>
+      <c r="BU73" s="8">
+        <v>5244</v>
       </c>
     </row>
-    <row r="74" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>302</v>
       </c>
       <c r="C74" s="6">
         <v>64</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E74" s="2">
         <v>3</v>
@@ -17631,22 +17684,22 @@
       <c r="BT74" s="2">
         <v>19.902999999999999</v>
       </c>
-      <c r="BU74" s="2">
-        <v>7.6999999999999999E-2</v>
+      <c r="BU74" s="8">
+        <v>7901</v>
       </c>
     </row>
-    <row r="75" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C75" s="6">
         <v>65</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E75" s="2">
         <v>3</v>
@@ -17843,25 +17896,25 @@
       <c r="BT75" s="2">
         <v>19.335999999999999</v>
       </c>
-      <c r="BU75" s="2">
-        <v>8.3000000000000004E-2</v>
+      <c r="BU75" s="8">
+        <v>8219</v>
       </c>
       <c r="BV75" s="2">
         <v>677</v>
       </c>
     </row>
-    <row r="76" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="C76" s="6">
         <v>66</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E76" s="2">
         <v>3</v>
@@ -18058,25 +18111,25 @@
       <c r="BT76" s="2">
         <v>19.004000000000001</v>
       </c>
-      <c r="BU76" s="2">
-        <v>0.11</v>
+      <c r="BU76" s="8">
+        <v>8551</v>
       </c>
       <c r="BV76" s="2">
         <v>500</v>
       </c>
     </row>
-    <row r="77" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>307</v>
       </c>
       <c r="C77" s="6">
         <v>67</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E77" s="2">
         <v>3</v>
@@ -18273,25 +18326,25 @@
       <c r="BT77" s="2">
         <v>18.753</v>
       </c>
-      <c r="BU77" s="2">
-        <v>0.11</v>
+      <c r="BU77" s="8">
+        <v>8795</v>
       </c>
       <c r="BV77" s="2">
         <v>746</v>
       </c>
     </row>
-    <row r="78" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C78" s="6">
         <v>68</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E78" s="2">
         <v>3</v>
@@ -18488,25 +18541,25 @@
       <c r="BT78" s="2">
         <v>18.449000000000002</v>
       </c>
-      <c r="BU78" s="2">
-        <v>0.12</v>
+      <c r="BU78" s="8">
+        <v>9066</v>
       </c>
       <c r="BV78" s="2">
         <v>814</v>
       </c>
     </row>
-    <row r="79" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C79" s="6">
         <v>69</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E79" s="2">
         <v>3</v>
@@ -18703,25 +18756,25 @@
       <c r="BT79" s="2">
         <v>18.126000000000001</v>
       </c>
-      <c r="BU79" s="2">
-        <v>0.14000000000000001</v>
+      <c r="BU79" s="8">
+        <v>9321</v>
       </c>
       <c r="BV79" s="2">
         <v>471</v>
       </c>
     </row>
-    <row r="80" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>311</v>
       </c>
       <c r="C80" s="6">
         <v>70</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E80" s="2">
         <v>1</v>
@@ -18921,25 +18974,25 @@
       <c r="BT80" s="2">
         <v>26.338999999999999</v>
       </c>
-      <c r="BU80" s="2">
-        <v>0.36</v>
+      <c r="BU80" s="8">
+        <v>6570</v>
       </c>
       <c r="BV80" s="2">
         <v>343</v>
       </c>
     </row>
-    <row r="81" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="C81" s="6">
         <v>71</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E81" s="2">
         <v>3</v>
@@ -19139,25 +19192,25 @@
       <c r="BT81" s="2">
         <v>17.779</v>
       </c>
-      <c r="BU81" s="2">
-        <v>0.18</v>
+      <c r="BU81" s="8">
+        <v>9841</v>
       </c>
       <c r="BV81" s="2">
         <v>893</v>
       </c>
     </row>
-    <row r="82" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="C82" s="6">
         <v>72</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E82" s="2">
         <v>3</v>
@@ -19357,25 +19410,25 @@
       <c r="BT82" s="2">
         <v>13.4102</v>
       </c>
-      <c r="BU82" s="2">
-        <v>0.33</v>
+      <c r="BU82" s="8">
+        <v>13310</v>
       </c>
       <c r="BV82" s="2">
         <v>1700</v>
       </c>
     </row>
-    <row r="83" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>317</v>
       </c>
       <c r="C83" s="6">
         <v>73</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E83" s="2">
         <v>2</v>
@@ -19575,25 +19628,25 @@
       <c r="BT83" s="2">
         <v>10.867699999999999</v>
       </c>
-      <c r="BU83" s="2">
-        <v>0.77</v>
+      <c r="BU83" s="8">
+        <v>16650</v>
       </c>
       <c r="BV83" s="2">
         <v>800</v>
       </c>
     </row>
-    <row r="84" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>318</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>319</v>
       </c>
       <c r="C84" s="6">
         <v>74</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E84" s="2">
         <v>2</v>
@@ -19793,25 +19846,25 @@
       <c r="BT84" s="2">
         <v>9.5501000000000005</v>
       </c>
-      <c r="BU84" s="2">
-        <v>2</v>
+      <c r="BU84" s="8">
+        <v>19250</v>
       </c>
       <c r="BV84" s="2">
         <v>2570</v>
       </c>
     </row>
-    <row r="85" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="C85" s="6">
         <v>75</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E85" s="2">
         <v>3</v>
@@ -20011,25 +20064,25 @@
       <c r="BT85" s="2">
         <v>8.8585600000000007</v>
       </c>
-      <c r="BU85" s="2">
-        <v>0.56000000000000005</v>
+      <c r="BU85" s="8">
+        <v>21020</v>
       </c>
       <c r="BV85" s="2">
         <v>1320</v>
       </c>
     </row>
-    <row r="86" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>322</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>323</v>
       </c>
       <c r="C86" s="6">
         <v>76</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E86" s="2">
         <v>3</v>
@@ -20223,25 +20276,25 @@
       <c r="BT86" s="2">
         <v>8.4209999999999994</v>
       </c>
-      <c r="BU86" s="2">
-        <v>1.2</v>
+      <c r="BU86" s="8">
+        <v>22590</v>
       </c>
       <c r="BV86" s="2">
         <v>3920</v>
       </c>
     </row>
-    <row r="87" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>325</v>
       </c>
       <c r="C87" s="6">
         <v>77</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E87" s="2">
         <v>1</v>
@@ -20441,25 +20494,25 @@
       <c r="BT87" s="2">
         <v>8.5203000000000007</v>
       </c>
-      <c r="BU87" s="2">
-        <v>2.1</v>
+      <c r="BU87" s="8">
+        <v>22560</v>
       </c>
       <c r="BV87" s="2">
         <v>1670</v>
       </c>
     </row>
-    <row r="88" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>327</v>
       </c>
       <c r="C88" s="6">
         <v>78</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E88" s="2">
         <v>1</v>
@@ -20659,25 +20712,25 @@
       <c r="BT88" s="2">
         <v>9.0947999999999993</v>
       </c>
-      <c r="BU88" s="2">
-        <v>0.94</v>
+      <c r="BU88" s="8">
+        <v>21090</v>
       </c>
       <c r="BV88" s="2">
         <v>392</v>
       </c>
     </row>
-    <row r="89" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>328</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>329</v>
       </c>
       <c r="C89" s="6">
         <v>79</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E89" s="2">
         <v>1</v>
@@ -20877,34 +20930,34 @@
       <c r="BT89" s="2">
         <v>10.210000000000001</v>
       </c>
-      <c r="BU89" s="2">
-        <v>4.5</v>
+      <c r="BU89" s="8">
+        <v>19300</v>
       </c>
       <c r="BV89" s="2">
         <v>2450</v>
       </c>
     </row>
-    <row r="90" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="C90" s="6">
         <v>80</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E90" s="2">
         <v>5</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I90" s="2">
         <v>3.0049999999999999</v>
@@ -21074,22 +21127,22 @@
       <c r="BT90" s="2">
         <v>14.821300000000001</v>
       </c>
-      <c r="BU90" s="2">
-        <v>0.1</v>
+      <c r="BU90" s="8">
+        <v>13534</v>
       </c>
     </row>
-    <row r="91" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B91" s="6" t="s">
         <v>333</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>334</v>
       </c>
       <c r="C91" s="6">
         <v>81</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E91" s="2">
         <v>3</v>
@@ -21292,25 +21345,25 @@
       <c r="BT91" s="2">
         <v>17.247299999999999</v>
       </c>
-      <c r="BU91" s="2">
-        <v>0.67</v>
+      <c r="BU91" s="8">
+        <v>11850</v>
       </c>
       <c r="BV91" s="2">
         <v>26.4</v>
       </c>
     </row>
-    <row r="92" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B92" s="6" t="s">
         <v>335</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>336</v>
       </c>
       <c r="C92" s="6">
         <v>82</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E92" s="2">
         <v>1</v>
@@ -21510,25 +21563,25 @@
       <c r="BT92" s="2">
         <v>18.271999999999998</v>
       </c>
-      <c r="BU92" s="2">
-        <v>0.48</v>
+      <c r="BU92" s="8">
+        <v>11340</v>
       </c>
       <c r="BV92" s="2">
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>337</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>338</v>
       </c>
       <c r="C93" s="6">
         <v>83</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E93" s="2">
         <v>7</v>
@@ -21722,31 +21775,31 @@
       <c r="BT93" s="2">
         <v>21.367999999999999</v>
       </c>
-      <c r="BU93" s="2">
-        <v>7.6999999999999999E-2</v>
+      <c r="BU93" s="8">
+        <v>9780</v>
       </c>
       <c r="BV93" s="2">
         <v>94.2</v>
       </c>
     </row>
-    <row r="94" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>340</v>
       </c>
       <c r="C94" s="6">
         <v>84</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I94" s="2">
         <v>3.359</v>
@@ -21895,22 +21948,22 @@
       <c r="BT94" s="2">
         <v>22.727272729999999</v>
       </c>
-      <c r="BU94" s="2">
-        <v>0.23</v>
+      <c r="BU94" s="8">
+        <v>9196</v>
       </c>
     </row>
-    <row r="95" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>342</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>343</v>
       </c>
       <c r="C95" s="6">
         <v>85</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M95" s="2">
         <v>1.27</v>
@@ -22026,19 +22079,20 @@
       <c r="BS95" s="2">
         <v>210</v>
       </c>
+      <c r="BU95" s="8"/>
     </row>
-    <row r="96" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>344</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>345</v>
       </c>
       <c r="C96" s="6">
         <v>86</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M96" s="2">
         <v>1.2</v>
@@ -22151,19 +22205,22 @@
       <c r="BT96" s="2">
         <v>22816.032889999999</v>
       </c>
+      <c r="BU96" s="8">
+        <v>9.73</v>
+      </c>
     </row>
-    <row r="97" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B97" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>347</v>
       </c>
       <c r="C97" s="6">
         <v>87</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="N97" s="2">
         <v>1.74</v>
@@ -22279,19 +22336,20 @@
       <c r="BS97" s="2">
         <v>223</v>
       </c>
+      <c r="BU97" s="8"/>
     </row>
-    <row r="98" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>348</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>349</v>
       </c>
       <c r="C98" s="6">
         <v>88</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I98" s="2">
         <v>5.1479999999999997</v>
@@ -22434,22 +22492,22 @@
       <c r="BT98" s="2">
         <v>45.2</v>
       </c>
-      <c r="BU98" s="2">
-        <v>0.1</v>
+      <c r="BU98" s="8">
+        <v>5000</v>
       </c>
     </row>
-    <row r="99" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B99" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="C99" s="6">
         <v>89</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I99" s="2">
         <v>5.67</v>
@@ -22586,19 +22644,22 @@
       <c r="BT99" s="2">
         <v>22.542204569999999</v>
       </c>
+      <c r="BU99" s="8">
+        <v>10070</v>
+      </c>
     </row>
-    <row r="100" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>352</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>353</v>
       </c>
       <c r="C100" s="6">
         <v>90</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I100" s="2">
         <v>5.0842000000000001</v>
@@ -22777,25 +22838,25 @@
       <c r="BT100" s="2">
         <v>19.791699999999999</v>
       </c>
-      <c r="BU100" s="2">
-        <v>0.67</v>
+      <c r="BU100" s="8">
+        <v>11724</v>
       </c>
       <c r="BV100" s="2">
         <v>400</v>
       </c>
     </row>
-    <row r="101" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B101" s="6" t="s">
         <v>354</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>355</v>
       </c>
       <c r="C101" s="6">
         <v>91</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I101" s="2">
         <v>3.9249999999999998</v>
@@ -22938,22 +22999,22 @@
       <c r="BT101" s="2">
         <v>15.031599999999999</v>
       </c>
-      <c r="BU101" s="2">
-        <v>0.56000000000000005</v>
+      <c r="BU101" s="8">
+        <v>15370</v>
       </c>
     </row>
-    <row r="102" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>356</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>357</v>
       </c>
       <c r="C102" s="6">
         <v>92</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I102" s="2">
         <v>2.8536999999999999</v>
@@ -23132,25 +23193,25 @@
       <c r="BT102" s="2">
         <v>12.494999999999999</v>
       </c>
-      <c r="BU102" s="2">
-        <v>0.36</v>
+      <c r="BU102" s="8">
+        <v>19050</v>
       </c>
       <c r="BV102" s="2">
         <v>2400</v>
       </c>
     </row>
-    <row r="103" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C103" s="6">
         <v>93</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I103" s="2">
         <v>6.6630000000000003</v>
@@ -23281,22 +23342,22 @@
       <c r="BT103" s="2">
         <v>11.589242049999999</v>
       </c>
-      <c r="BU103" s="2">
-        <v>8.3000000000000004E-2</v>
+      <c r="BU103" s="8">
+        <v>20450</v>
       </c>
     </row>
-    <row r="104" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>359</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>360</v>
       </c>
       <c r="C104" s="6">
         <v>94</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I104" s="2">
         <v>6.1829999999999998</v>
@@ -23448,22 +23509,22 @@
       <c r="BT104" s="2">
         <v>12.3132822</v>
       </c>
-      <c r="BU104" s="2">
-        <v>6.7000000000000004E-2</v>
+      <c r="BU104" s="8">
+        <v>19816</v>
       </c>
     </row>
-    <row r="105" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>361</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>362</v>
       </c>
       <c r="C105" s="6">
         <v>95</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I105" s="2">
         <v>3.4681000000000002</v>
@@ -23576,19 +23637,22 @@
       <c r="BT105" s="2">
         <v>17.776152159999999</v>
       </c>
+      <c r="BU105" s="8">
+        <v>13670</v>
+      </c>
     </row>
-    <row r="106" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>364</v>
       </c>
       <c r="C106" s="6">
         <v>96</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I106" s="2">
         <v>3.496</v>
@@ -23698,19 +23762,22 @@
       <c r="BT106" s="2">
         <v>18.28275352</v>
       </c>
+      <c r="BU106" s="8">
+        <v>13510</v>
+      </c>
     </row>
-    <row r="107" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="B107" s="6" t="s">
         <v>365</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>366</v>
       </c>
       <c r="C107" s="6">
         <v>97</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I107" s="2">
         <v>3.4159999999999999</v>
@@ -23817,19 +23884,22 @@
       <c r="BT107" s="2">
         <v>16.711772669999998</v>
       </c>
+      <c r="BU107" s="8">
+        <v>14780</v>
+      </c>
     </row>
-    <row r="108" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>367</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>368</v>
       </c>
       <c r="C108" s="6">
         <v>98</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I108" s="2">
         <v>3.38</v>
@@ -23936,19 +24006,22 @@
       <c r="BT108" s="2">
         <v>16.622516560000001</v>
       </c>
+      <c r="BU108" s="8">
+        <v>15100</v>
+      </c>
     </row>
-    <row r="109" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C109" s="6">
         <v>99</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N109" s="2">
         <v>0.98</v>
@@ -24043,19 +24116,20 @@
       <c r="BS109" s="2">
         <v>252</v>
       </c>
+      <c r="BU109" s="8"/>
     </row>
-    <row r="110" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:74" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="B110" s="6" t="s">
         <v>370</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>371</v>
       </c>
       <c r="C110" s="6">
         <v>100</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N110" s="2">
         <v>0.97</v>
@@ -24150,6 +24224,43 @@
       <c r="BS110" s="2">
         <v>257</v>
       </c>
+      <c r="BU110" s="8"/>
+    </row>
+    <row r="111" spans="1:74" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU111" s="8"/>
+    </row>
+    <row r="112" spans="1:74" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU112" s="8"/>
+    </row>
+    <row r="113" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU113" s="8"/>
+    </row>
+    <row r="114" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU114" s="8"/>
+    </row>
+    <row r="115" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU115" s="8"/>
+    </row>
+    <row r="116" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU116" s="8"/>
+    </row>
+    <row r="117" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU117" s="8"/>
+    </row>
+    <row r="118" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU118" s="8"/>
+    </row>
+    <row r="119" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU119" s="8"/>
+    </row>
+    <row r="120" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU120" s="8"/>
+    </row>
+    <row r="121" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU121" s="8"/>
+    </row>
+    <row r="122" spans="73:73" ht="15" x14ac:dyDescent="0.2">
+      <c r="BU122" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>